<commit_message>
Modified my schedule and added new school schedule.
</commit_message>
<xml_diff>
--- a/2018-2019 2nd semester.xlsx
+++ b/2018-2019 2nd semester.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\MySchedule\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A310575-6746-4B77-95F4-DF662C83DC60}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75092230-3676-4100-A513-DA8F93ABCE3F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="100">
   <si>
     <t/>
   </si>
@@ -285,10 +285,6 @@
     <t>DG3</t>
   </si>
   <si>
-    <t>DG3</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
     <t>SD5</t>
   </si>
   <si>
@@ -320,7 +316,7 @@
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">1-电工技术与电子技术C(56/3.5)(220160/刘锐/讲师)_x000D_
+    <t>1-电工技术与电子技术C(56/3.5)(220160/刘锐/讲师)_x000D_
 材料2017-1班;材料2017-2班;材料2017-3班_x000D_
 2-通信原理A(64/4.0)(220160/刘锐/讲师)_x000D_
 信息2016-01班;信息2016-02班_x000D_
@@ -334,7 +330,20 @@
 SD7--自动化17-3
 SD10--电气17-3
 SD12--电气17-5
-</t>
+TX1--信息16-1
+TX2--信息16-2</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>TX2</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>TX1</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>DG1,2/3</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
 </sst>
@@ -1059,7 +1068,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1097,9 +1106,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1118,6 +1124,18 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="28" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1127,12 +1145,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1148,13 +1160,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1516,7 +1528,7 @@
   <dimension ref="A1:X47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+      <selection activeCell="R19" sqref="R19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1525,8 +1537,7 @@
     <col min="2" max="10" width="6" customWidth="1"/>
     <col min="11" max="11" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="6" customWidth="1"/>
-    <col min="13" max="13" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="6" customWidth="1"/>
     <col min="16" max="20" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="21" max="22" width="6" customWidth="1"/>
@@ -1535,62 +1546,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-      <c r="N1" s="21"/>
-      <c r="O1" s="21"/>
-      <c r="P1" s="21"/>
-      <c r="Q1" s="21"/>
-      <c r="R1" s="21"/>
-      <c r="S1" s="21"/>
-      <c r="T1" s="21"/>
-      <c r="U1" s="21"/>
-      <c r="V1" s="21"/>
-      <c r="W1" s="21"/>
-      <c r="X1" s="21"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
+      <c r="P1" s="24"/>
+      <c r="Q1" s="24"/>
+      <c r="R1" s="24"/>
+      <c r="S1" s="24"/>
+      <c r="T1" s="24"/>
+      <c r="U1" s="24"/>
+      <c r="V1" s="24"/>
+      <c r="W1" s="24"/>
+      <c r="X1" s="24"/>
     </row>
     <row r="2" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="29" t="s">
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="N2" s="21"/>
-      <c r="O2" s="21"/>
-      <c r="P2" s="21"/>
-      <c r="Q2" s="21"/>
-      <c r="R2" s="21"/>
-      <c r="S2" s="21"/>
-      <c r="T2" s="21"/>
-      <c r="U2" s="21"/>
-      <c r="V2" s="21"/>
-      <c r="W2" s="21"/>
-      <c r="X2" s="21"/>
+      <c r="N2" s="24"/>
+      <c r="O2" s="24"/>
+      <c r="P2" s="24"/>
+      <c r="Q2" s="24"/>
+      <c r="R2" s="24"/>
+      <c r="S2" s="24"/>
+      <c r="T2" s="24"/>
+      <c r="U2" s="24"/>
+      <c r="V2" s="24"/>
+      <c r="W2" s="24"/>
+      <c r="X2" s="24"/>
     </row>
     <row r="3" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -1741,7 +1752,7 @@
       </c>
     </row>
     <row r="5" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="24" t="s">
         <v>49</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1768,24 +1779,22 @@
       <c r="I5" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="J5" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="K5" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="L5" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="M5" s="12" t="s">
-        <v>87</v>
-      </c>
+      <c r="J5" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="K5" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="L5" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="M5" s="10"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
-      <c r="S5" s="21" t="s">
+      <c r="S5" s="24" t="s">
         <v>70</v>
       </c>
       <c r="T5" s="1"/>
@@ -1794,104 +1803,100 @@
       <c r="W5" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="X5" s="22" t="s">
-        <v>97</v>
+      <c r="X5" s="25" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="21"/>
+      <c r="A6" s="24"/>
       <c r="B6" s="1" t="s">
         <v>51</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
-      <c r="E6" s="19" t="s">
+      <c r="E6" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="F6" s="19" t="s">
+      <c r="F6" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="G6" s="19" t="s">
+      <c r="G6" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="H6" s="19" t="s">
+      <c r="H6" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="I6" s="19" t="s">
+      <c r="I6" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="J6" s="13" t="s">
+      <c r="J6" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="K6" s="13" t="s">
+      <c r="K6" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="L6" s="14"/>
-      <c r="M6" s="13" t="s">
-        <v>80</v>
-      </c>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
-      <c r="S6" s="21" t="s">
+      <c r="S6" s="24" t="s">
         <v>0</v>
       </c>
       <c r="T6" s="1"/>
       <c r="U6" s="1"/>
       <c r="V6" s="1"/>
       <c r="W6" s="1"/>
-      <c r="X6" s="21"/>
+      <c r="X6" s="24"/>
     </row>
     <row r="7" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="21"/>
+      <c r="A7" s="24"/>
       <c r="B7" s="1" t="s">
         <v>52</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
-      <c r="E7" s="19" t="s">
+      <c r="E7" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="F7" s="19" t="s">
+      <c r="F7" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="G7" s="19" t="s">
+      <c r="G7" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="H7" s="19" t="s">
+      <c r="H7" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="I7" s="19" t="s">
+      <c r="I7" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="J7" s="13" t="s">
+      <c r="J7" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="K7" s="13" t="s">
+      <c r="K7" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="L7" s="14"/>
-      <c r="M7" s="13" t="s">
-        <v>82</v>
-      </c>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
-      <c r="S7" s="21" t="s">
+      <c r="S7" s="24" t="s">
         <v>0</v>
       </c>
       <c r="T7" s="1"/>
       <c r="U7" s="1"/>
       <c r="V7" s="1"/>
       <c r="W7" s="1"/>
-      <c r="X7" s="21"/>
+      <c r="X7" s="24"/>
     </row>
     <row r="8" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="21"/>
+      <c r="A8" s="24"/>
       <c r="B8" s="1" t="s">
         <v>53</v>
       </c>
@@ -1914,24 +1919,21 @@
       <c r="I8" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="J8" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="K8" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="L8" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="M8" s="18" t="s">
-        <v>92</v>
+      <c r="J8" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="K8" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="M8" s="33" t="s">
+        <v>91</v>
       </c>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
-      <c r="S8" s="21" t="s">
+      <c r="S8" s="24" t="s">
         <v>0</v>
       </c>
       <c r="T8" s="1"/>
@@ -1940,10 +1942,10 @@
       <c r="W8" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="X8" s="21"/>
+      <c r="X8" s="24"/>
     </row>
     <row r="9" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="21"/>
+      <c r="A9" s="24"/>
       <c r="B9" s="1" t="s">
         <v>54</v>
       </c>
@@ -1957,25 +1959,23 @@
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
-      <c r="M9" s="23" t="s">
-        <v>85</v>
-      </c>
+      <c r="M9" s="22"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
-      <c r="S9" s="21" t="s">
+      <c r="S9" s="24" t="s">
         <v>0</v>
       </c>
       <c r="T9" s="1"/>
       <c r="U9" s="1"/>
       <c r="V9" s="1"/>
       <c r="W9" s="1"/>
-      <c r="X9" s="21"/>
+      <c r="X9" s="24"/>
     </row>
     <row r="10" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="21"/>
+      <c r="A10" s="24"/>
       <c r="B10" s="1" t="s">
         <v>55</v>
       </c>
@@ -1989,23 +1989,23 @@
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
-      <c r="M10" s="24"/>
+      <c r="M10" s="22"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
-      <c r="S10" s="21" t="s">
+      <c r="S10" s="24" t="s">
         <v>0</v>
       </c>
       <c r="T10" s="1"/>
       <c r="U10" s="1"/>
       <c r="V10" s="1"/>
       <c r="W10" s="1"/>
-      <c r="X10" s="21"/>
+      <c r="X10" s="24"/>
     </row>
     <row r="11" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="21" t="s">
+      <c r="A11" s="24" t="s">
         <v>56</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -2013,27 +2013,29 @@
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="25" t="s">
+      <c r="E11" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="F11" s="25" t="s">
+      <c r="F11" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="G11" s="25" t="s">
+      <c r="G11" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="H11" s="25" t="s">
+      <c r="H11" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="23" t="s">
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="L11" s="21" t="s">
+      <c r="L11" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="M11" s="1"/>
+      <c r="M11" s="12" t="s">
+        <v>98</v>
+      </c>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
@@ -2044,23 +2046,23 @@
       <c r="U11" s="1"/>
       <c r="V11" s="1"/>
       <c r="W11" s="1"/>
-      <c r="X11" s="21"/>
+      <c r="X11" s="24"/>
     </row>
     <row r="12" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="21"/>
+      <c r="A12" s="24"/>
       <c r="B12" s="1" t="s">
         <v>51</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="26"/>
-      <c r="H12" s="26"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="24"/>
-      <c r="L12" s="21" t="s">
+      <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="27"/>
+      <c r="L12" s="24" t="s">
         <v>0</v>
       </c>
       <c r="M12" s="1"/>
@@ -2074,55 +2076,57 @@
       <c r="U12" s="1"/>
       <c r="V12" s="1"/>
       <c r="W12" s="1"/>
-      <c r="X12" s="21"/>
+      <c r="X12" s="24"/>
     </row>
     <row r="13" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="21"/>
+      <c r="A13" s="24"/>
       <c r="B13" s="1" t="s">
         <v>52</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
-      <c r="L13" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="M13" s="1"/>
-      <c r="O13" s="18" t="s">
-        <v>93</v>
-      </c>
-      <c r="P13" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="Q13" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="R13" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="S13" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="T13" s="18" t="s">
-        <v>95</v>
+      <c r="L13" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="M13" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="O13" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="P13" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q13" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="R13" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="S13" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="T13" s="17" t="s">
+        <v>94</v>
       </c>
       <c r="U13" s="1"/>
       <c r="V13" s="1"/>
       <c r="W13" s="1"/>
-      <c r="X13" s="21"/>
+      <c r="X13" s="24"/>
     </row>
     <row r="14" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="21"/>
+      <c r="A14" s="24"/>
       <c r="B14" s="1" t="s">
         <v>53</v>
       </c>
@@ -2135,7 +2139,7 @@
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
-      <c r="L14" s="21" t="s">
+      <c r="L14" s="24" t="s">
         <v>0</v>
       </c>
       <c r="M14" s="1"/>
@@ -2149,10 +2153,10 @@
       <c r="U14" s="1"/>
       <c r="V14" s="1"/>
       <c r="W14" s="1"/>
-      <c r="X14" s="21"/>
+      <c r="X14" s="24"/>
     </row>
     <row r="15" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="21"/>
+      <c r="A15" s="24"/>
       <c r="B15" s="1" t="s">
         <v>54</v>
       </c>
@@ -2165,10 +2169,12 @@
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
-      <c r="L15" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="M15" s="1"/>
+      <c r="L15" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="M15" s="31" t="s">
+        <v>99</v>
+      </c>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
@@ -2179,10 +2185,10 @@
       <c r="U15" s="1"/>
       <c r="V15" s="1"/>
       <c r="W15" s="1"/>
-      <c r="X15" s="21"/>
+      <c r="X15" s="24"/>
     </row>
     <row r="16" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="21"/>
+      <c r="A16" s="24"/>
       <c r="B16" s="1" t="s">
         <v>55</v>
       </c>
@@ -2195,10 +2201,10 @@
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
-      <c r="L16" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="M16" s="1"/>
+      <c r="L16" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="M16" s="32"/>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
@@ -2209,10 +2215,10 @@
       <c r="U16" s="1"/>
       <c r="V16" s="1"/>
       <c r="W16" s="1"/>
-      <c r="X16" s="21"/>
+      <c r="X16" s="24"/>
     </row>
     <row r="17" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="21" t="s">
+      <c r="A17" s="24" t="s">
         <v>57</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -2234,16 +2240,16 @@
       <c r="H17" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="I17" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="J17" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="K17" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="L17" s="21" t="s">
+      <c r="I17" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="J17" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="K17" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="L17" s="24" t="s">
         <v>0</v>
       </c>
       <c r="M17" s="11" t="s">
@@ -2261,10 +2267,10 @@
       <c r="W17" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="X17" s="21"/>
+      <c r="X17" s="24"/>
     </row>
     <row r="18" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="21"/>
+      <c r="A18" s="24"/>
       <c r="B18" s="1" t="s">
         <v>51</v>
       </c>
@@ -2275,42 +2281,46 @@
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="M18" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="N18" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="O18" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="P18" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="Q18" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="R18" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="S18" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="T18" s="18" t="s">
-        <v>94</v>
+      <c r="J18" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="K18" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="L18" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="M18" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="N18" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="O18" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="P18" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q18" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="R18" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="S18" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="T18" s="17" t="s">
+        <v>93</v>
       </c>
       <c r="U18" s="1"/>
       <c r="V18" s="1"/>
       <c r="W18" s="1"/>
-      <c r="X18" s="21"/>
+      <c r="X18" s="24"/>
     </row>
     <row r="19" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="21"/>
+      <c r="A19" s="24"/>
       <c r="B19" s="1" t="s">
         <v>52</v>
       </c>
@@ -2323,28 +2333,28 @@
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
-      <c r="L19" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="M19" s="17"/>
-      <c r="N19" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="O19" s="17"/>
-      <c r="P19" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="Q19" s="17"/>
-      <c r="R19" s="17"/>
-      <c r="S19" s="17"/>
-      <c r="T19" s="17"/>
+      <c r="L19" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="M19" s="16"/>
+      <c r="N19" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="O19" s="16"/>
+      <c r="P19" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q19" s="16"/>
+      <c r="R19" s="16"/>
+      <c r="S19" s="16"/>
+      <c r="T19" s="16"/>
       <c r="U19" s="1"/>
       <c r="V19" s="1"/>
       <c r="W19" s="1"/>
-      <c r="X19" s="21"/>
+      <c r="X19" s="24"/>
     </row>
     <row r="20" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="21"/>
+      <c r="A20" s="24"/>
       <c r="B20" s="1" t="s">
         <v>53</v>
       </c>
@@ -2366,16 +2376,16 @@
       <c r="H20" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="I20" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="J20" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="K20" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="L20" s="21" t="s">
+      <c r="I20" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="J20" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="K20" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="L20" s="24" t="s">
         <v>0</v>
       </c>
       <c r="M20" s="1"/>
@@ -2391,10 +2401,10 @@
       <c r="W20" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="X20" s="21"/>
+      <c r="X20" s="24"/>
     </row>
     <row r="21" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="21"/>
+      <c r="A21" s="24"/>
       <c r="B21" s="1" t="s">
         <v>54</v>
       </c>
@@ -2407,7 +2417,7 @@
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
-      <c r="L21" s="21" t="s">
+      <c r="L21" s="24" t="s">
         <v>0</v>
       </c>
       <c r="M21" s="1"/>
@@ -2421,10 +2431,10 @@
       <c r="U21" s="1"/>
       <c r="V21" s="1"/>
       <c r="W21" s="1"/>
-      <c r="X21" s="21"/>
+      <c r="X21" s="24"/>
     </row>
     <row r="22" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="21"/>
+      <c r="A22" s="24"/>
       <c r="B22" s="1" t="s">
         <v>55</v>
       </c>
@@ -2437,7 +2447,7 @@
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
-      <c r="L22" s="21" t="s">
+      <c r="L22" s="24" t="s">
         <v>0</v>
       </c>
       <c r="M22" s="1"/>
@@ -2451,10 +2461,10 @@
       <c r="U22" s="1"/>
       <c r="V22" s="1"/>
       <c r="W22" s="1"/>
-      <c r="X22" s="21"/>
+      <c r="X22" s="24"/>
     </row>
     <row r="23" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="21" t="s">
+      <c r="A23" s="24" t="s">
         <v>58</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -2467,30 +2477,36 @@
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="M23" s="30" t="s">
+      <c r="J23" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="K23" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="L23" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="M23" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="N23" s="31"/>
-      <c r="O23" s="31"/>
-      <c r="P23" s="31"/>
-      <c r="Q23" s="31"/>
-      <c r="R23" s="31"/>
-      <c r="S23" s="31"/>
-      <c r="T23" s="31"/>
-      <c r="U23" s="31"/>
-      <c r="V23" s="31"/>
-      <c r="W23" s="31" t="s">
+      <c r="N23" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="O23" s="20"/>
+      <c r="P23" s="20"/>
+      <c r="Q23" s="20"/>
+      <c r="R23" s="20"/>
+      <c r="S23" s="20"/>
+      <c r="T23" s="20"/>
+      <c r="U23" s="20"/>
+      <c r="V23" s="20"/>
+      <c r="W23" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="X23" s="21"/>
+      <c r="X23" s="24"/>
     </row>
     <row r="24" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="21"/>
+      <c r="A24" s="24"/>
       <c r="B24" s="1" t="s">
         <v>51</v>
       </c>
@@ -2510,51 +2526,51 @@
         <v>64</v>
       </c>
       <c r="H24" s="10"/>
-      <c r="I24" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="J24" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="K24" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="L24" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="M24" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="N24" s="18" t="s">
+      <c r="I24" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="J24" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="K24" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="L24" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="M24" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="O24" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="P24" s="18" t="s">
+      <c r="N24" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="O24" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="Q24" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="R24" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="S24" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="T24" s="18" t="s">
-        <v>91</v>
+      <c r="P24" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q24" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="R24" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="S24" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="T24" s="17" t="s">
+        <v>90</v>
       </c>
       <c r="U24" s="1"/>
       <c r="V24" s="1"/>
       <c r="W24" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="X24" s="21"/>
+      <c r="X24" s="24"/>
     </row>
     <row r="25" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="21"/>
+      <c r="A25" s="24"/>
       <c r="B25" s="1" t="s">
         <v>52</v>
       </c>
@@ -2567,7 +2583,7 @@
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
-      <c r="L25" s="21" t="s">
+      <c r="L25" s="24" t="s">
         <v>0</v>
       </c>
       <c r="M25" s="1"/>
@@ -2581,10 +2597,10 @@
       <c r="U25" s="1"/>
       <c r="V25" s="1"/>
       <c r="W25" s="1"/>
-      <c r="X25" s="21"/>
+      <c r="X25" s="24"/>
     </row>
     <row r="26" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="21"/>
+      <c r="A26" s="24"/>
       <c r="B26" s="1" t="s">
         <v>53</v>
       </c>
@@ -2602,70 +2618,70 @@
         <v>64</v>
       </c>
       <c r="H26" s="10"/>
-      <c r="I26" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="J26" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="K26" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="L26" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="M26" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="N26" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="O26" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="P26" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="Q26" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="R26" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="S26" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="T26" s="18" t="s">
-        <v>89</v>
+      <c r="I26" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="J26" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="K26" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="L26" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="M26" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="N26" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="O26" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="P26" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q26" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="R26" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="S26" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="T26" s="17" t="s">
+        <v>88</v>
       </c>
       <c r="U26" s="1"/>
       <c r="V26" s="1"/>
       <c r="W26" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="X26" s="21"/>
+      <c r="X26" s="24"/>
     </row>
     <row r="27" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="21"/>
+      <c r="A27" s="24"/>
       <c r="B27" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
-      <c r="E27" s="25" t="s">
+      <c r="E27" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="F27" s="15"/>
-      <c r="G27" s="25" t="s">
+      <c r="F27" s="14"/>
+      <c r="G27" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="H27" s="15"/>
-      <c r="I27" s="15"/>
-      <c r="J27" s="23" t="s">
+      <c r="H27" s="14"/>
+      <c r="I27" s="14"/>
+      <c r="J27" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="K27" s="15"/>
-      <c r="L27" s="21" t="s">
+      <c r="K27" s="14"/>
+      <c r="L27" s="24" t="s">
         <v>0</v>
       </c>
       <c r="M27" s="1"/>
@@ -2679,23 +2695,23 @@
       <c r="U27" s="1"/>
       <c r="V27" s="1"/>
       <c r="W27" s="1"/>
-      <c r="X27" s="21"/>
+      <c r="X27" s="24"/>
     </row>
     <row r="28" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="21"/>
+      <c r="A28" s="24"/>
       <c r="B28" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
-      <c r="E28" s="26"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="26"/>
-      <c r="H28" s="16"/>
-      <c r="I28" s="16"/>
-      <c r="J28" s="24"/>
-      <c r="K28" s="15"/>
-      <c r="L28" s="21" t="s">
+      <c r="E28" s="27"/>
+      <c r="F28" s="14"/>
+      <c r="G28" s="27"/>
+      <c r="H28" s="15"/>
+      <c r="I28" s="15"/>
+      <c r="J28" s="27"/>
+      <c r="K28" s="14"/>
+      <c r="L28" s="24" t="s">
         <v>0</v>
       </c>
       <c r="M28" s="1"/>
@@ -2709,10 +2725,10 @@
       <c r="U28" s="1"/>
       <c r="V28" s="1"/>
       <c r="W28" s="1"/>
-      <c r="X28" s="21"/>
+      <c r="X28" s="24"/>
     </row>
     <row r="29" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="21" t="s">
+      <c r="A29" s="24" t="s">
         <v>59</v>
       </c>
       <c r="B29" s="1" t="s">
@@ -2723,10 +2739,10 @@
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
-      <c r="H29" s="21" t="s">
+      <c r="H29" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="I29" s="11" t="s">
+      <c r="I29" s="9" t="s">
         <v>63</v>
       </c>
       <c r="J29" s="1"/>
@@ -2736,7 +2752,7 @@
       <c r="N29" s="1"/>
       <c r="O29" s="1"/>
       <c r="P29" s="1"/>
-      <c r="Q29" s="21" t="s">
+      <c r="Q29" s="24" t="s">
         <v>69</v>
       </c>
       <c r="R29" s="1"/>
@@ -2744,13 +2760,13 @@
       <c r="T29" s="1"/>
       <c r="U29" s="1"/>
       <c r="V29" s="1"/>
-      <c r="W29" s="32" t="s">
+      <c r="W29" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="X29" s="21"/>
+      <c r="X29" s="24"/>
     </row>
     <row r="30" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="21"/>
+      <c r="A30" s="24"/>
       <c r="B30" s="1" t="s">
         <v>51</v>
       </c>
@@ -2759,7 +2775,7 @@
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
-      <c r="H30" s="21" t="s">
+      <c r="H30" s="24" t="s">
         <v>0</v>
       </c>
       <c r="I30" s="1"/>
@@ -2770,7 +2786,7 @@
       <c r="N30" s="1"/>
       <c r="O30" s="1"/>
       <c r="P30" s="1"/>
-      <c r="Q30" s="21" t="s">
+      <c r="Q30" s="24" t="s">
         <v>0</v>
       </c>
       <c r="R30" s="1"/>
@@ -2779,10 +2795,10 @@
       <c r="U30" s="1"/>
       <c r="V30" s="1"/>
       <c r="W30" s="1"/>
-      <c r="X30" s="21"/>
+      <c r="X30" s="24"/>
     </row>
     <row r="31" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="21"/>
+      <c r="A31" s="24"/>
       <c r="B31" s="1" t="s">
         <v>52</v>
       </c>
@@ -2791,7 +2807,7 @@
       <c r="E31" s="10"/>
       <c r="F31" s="10"/>
       <c r="G31" s="10"/>
-      <c r="H31" s="21" t="s">
+      <c r="H31" s="24" t="s">
         <v>0</v>
       </c>
       <c r="I31" s="10"/>
@@ -2802,7 +2818,7 @@
       <c r="N31" s="1"/>
       <c r="O31" s="1"/>
       <c r="P31" s="1"/>
-      <c r="Q31" s="21" t="s">
+      <c r="Q31" s="24" t="s">
         <v>0</v>
       </c>
       <c r="R31" s="1"/>
@@ -2811,10 +2827,10 @@
       <c r="U31" s="1"/>
       <c r="V31" s="1"/>
       <c r="W31" s="1"/>
-      <c r="X31" s="21"/>
+      <c r="X31" s="24"/>
     </row>
     <row r="32" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="21"/>
+      <c r="A32" s="24"/>
       <c r="B32" s="1" t="s">
         <v>53</v>
       </c>
@@ -2823,7 +2839,7 @@
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
-      <c r="H32" s="21" t="s">
+      <c r="H32" s="24" t="s">
         <v>0</v>
       </c>
       <c r="I32" s="1"/>
@@ -2833,7 +2849,7 @@
       <c r="N32" s="1"/>
       <c r="O32" s="1"/>
       <c r="P32" s="1"/>
-      <c r="Q32" s="21" t="s">
+      <c r="Q32" s="24" t="s">
         <v>0</v>
       </c>
       <c r="R32" s="1"/>
@@ -2842,10 +2858,10 @@
       <c r="U32" s="1"/>
       <c r="V32" s="1"/>
       <c r="W32" s="1"/>
-      <c r="X32" s="21"/>
+      <c r="X32" s="24"/>
     </row>
     <row r="33" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="21"/>
+      <c r="A33" s="24"/>
       <c r="B33" s="1" t="s">
         <v>54</v>
       </c>
@@ -2854,7 +2870,7 @@
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
-      <c r="H33" s="21" t="s">
+      <c r="H33" s="24" t="s">
         <v>0</v>
       </c>
       <c r="I33" s="1"/>
@@ -2865,7 +2881,7 @@
       <c r="N33" s="1"/>
       <c r="O33" s="1"/>
       <c r="P33" s="1"/>
-      <c r="Q33" s="21" t="s">
+      <c r="Q33" s="24" t="s">
         <v>0</v>
       </c>
       <c r="R33" s="1"/>
@@ -2874,10 +2890,10 @@
       <c r="U33" s="1"/>
       <c r="V33" s="1"/>
       <c r="W33" s="1"/>
-      <c r="X33" s="21"/>
+      <c r="X33" s="24"/>
     </row>
     <row r="34" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="21"/>
+      <c r="A34" s="24"/>
       <c r="B34" s="1" t="s">
         <v>55</v>
       </c>
@@ -2886,7 +2902,7 @@
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
-      <c r="H34" s="21" t="s">
+      <c r="H34" s="24" t="s">
         <v>0</v>
       </c>
       <c r="I34" s="1"/>
@@ -2897,7 +2913,7 @@
       <c r="N34" s="1"/>
       <c r="O34" s="1"/>
       <c r="P34" s="1"/>
-      <c r="Q34" s="21" t="s">
+      <c r="Q34" s="24" t="s">
         <v>0</v>
       </c>
       <c r="R34" s="1"/>
@@ -2906,10 +2922,10 @@
       <c r="U34" s="1"/>
       <c r="V34" s="1"/>
       <c r="W34" s="1"/>
-      <c r="X34" s="21"/>
+      <c r="X34" s="24"/>
     </row>
     <row r="35" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="21" t="s">
+      <c r="A35" s="24" t="s">
         <v>60</v>
       </c>
       <c r="B35" s="1" t="s">
@@ -2920,7 +2936,7 @@
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
-      <c r="H35" s="21" t="s">
+      <c r="H35" s="24" t="s">
         <v>0</v>
       </c>
       <c r="I35" s="1"/>
@@ -2930,10 +2946,10 @@
       <c r="M35" s="1"/>
       <c r="N35" s="1"/>
       <c r="O35" s="1"/>
-      <c r="P35" s="21" t="s">
+      <c r="P35" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="Q35" s="21" t="s">
+      <c r="Q35" s="24" t="s">
         <v>0</v>
       </c>
       <c r="R35" s="1"/>
@@ -2942,10 +2958,10 @@
       <c r="U35" s="1"/>
       <c r="V35" s="1"/>
       <c r="W35" s="1"/>
-      <c r="X35" s="21"/>
+      <c r="X35" s="24"/>
     </row>
     <row r="36" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="21"/>
+      <c r="A36" s="24"/>
       <c r="B36" s="1" t="s">
         <v>51</v>
       </c>
@@ -2954,7 +2970,7 @@
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
-      <c r="H36" s="21" t="s">
+      <c r="H36" s="24" t="s">
         <v>0</v>
       </c>
       <c r="I36" s="1"/>
@@ -2964,10 +2980,10 @@
       <c r="M36" s="1"/>
       <c r="N36" s="1"/>
       <c r="O36" s="1"/>
-      <c r="P36" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q36" s="21" t="s">
+      <c r="P36" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q36" s="24" t="s">
         <v>0</v>
       </c>
       <c r="R36" s="1"/>
@@ -2976,10 +2992,10 @@
       <c r="U36" s="1"/>
       <c r="V36" s="1"/>
       <c r="W36" s="1"/>
-      <c r="X36" s="21"/>
+      <c r="X36" s="24"/>
     </row>
     <row r="37" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="21"/>
+      <c r="A37" s="24"/>
       <c r="B37" s="1" t="s">
         <v>52</v>
       </c>
@@ -2988,7 +3004,7 @@
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
-      <c r="H37" s="21" t="s">
+      <c r="H37" s="24" t="s">
         <v>0</v>
       </c>
       <c r="I37" s="1"/>
@@ -2998,10 +3014,10 @@
       <c r="M37" s="1"/>
       <c r="N37" s="1"/>
       <c r="O37" s="1"/>
-      <c r="P37" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q37" s="21" t="s">
+      <c r="P37" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q37" s="24" t="s">
         <v>0</v>
       </c>
       <c r="R37" s="1"/>
@@ -3010,10 +3026,10 @@
       <c r="U37" s="1"/>
       <c r="V37" s="1"/>
       <c r="W37" s="1"/>
-      <c r="X37" s="21"/>
+      <c r="X37" s="24"/>
     </row>
     <row r="38" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="21"/>
+      <c r="A38" s="24"/>
       <c r="B38" s="1" t="s">
         <v>53</v>
       </c>
@@ -3022,7 +3038,7 @@
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
-      <c r="H38" s="21" t="s">
+      <c r="H38" s="24" t="s">
         <v>0</v>
       </c>
       <c r="I38" s="1"/>
@@ -3032,10 +3048,10 @@
       <c r="M38" s="1"/>
       <c r="N38" s="1"/>
       <c r="O38" s="1"/>
-      <c r="P38" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q38" s="21" t="s">
+      <c r="P38" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q38" s="24" t="s">
         <v>0</v>
       </c>
       <c r="R38" s="1"/>
@@ -3044,10 +3060,10 @@
       <c r="U38" s="1"/>
       <c r="V38" s="1"/>
       <c r="W38" s="1"/>
-      <c r="X38" s="21"/>
+      <c r="X38" s="24"/>
     </row>
     <row r="39" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="21"/>
+      <c r="A39" s="24"/>
       <c r="B39" s="1" t="s">
         <v>54</v>
       </c>
@@ -3056,7 +3072,7 @@
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
-      <c r="H39" s="21" t="s">
+      <c r="H39" s="24" t="s">
         <v>0</v>
       </c>
       <c r="I39" s="1"/>
@@ -3066,10 +3082,10 @@
       <c r="M39" s="1"/>
       <c r="N39" s="1"/>
       <c r="O39" s="1"/>
-      <c r="P39" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q39" s="21" t="s">
+      <c r="P39" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q39" s="24" t="s">
         <v>0</v>
       </c>
       <c r="R39" s="1"/>
@@ -3078,10 +3094,10 @@
       <c r="U39" s="1"/>
       <c r="V39" s="1"/>
       <c r="W39" s="1"/>
-      <c r="X39" s="21"/>
+      <c r="X39" s="24"/>
     </row>
     <row r="40" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="21"/>
+      <c r="A40" s="24"/>
       <c r="B40" s="1" t="s">
         <v>55</v>
       </c>
@@ -3090,7 +3106,7 @@
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
-      <c r="H40" s="21" t="s">
+      <c r="H40" s="24" t="s">
         <v>0</v>
       </c>
       <c r="I40" s="1"/>
@@ -3100,10 +3116,10 @@
       <c r="M40" s="1"/>
       <c r="N40" s="1"/>
       <c r="O40" s="1"/>
-      <c r="P40" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q40" s="21" t="s">
+      <c r="P40" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q40" s="24" t="s">
         <v>0</v>
       </c>
       <c r="R40" s="1"/>
@@ -3112,10 +3128,10 @@
       <c r="U40" s="1"/>
       <c r="V40" s="1"/>
       <c r="W40" s="1"/>
-      <c r="X40" s="21"/>
+      <c r="X40" s="24"/>
     </row>
     <row r="41" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="21" t="s">
+      <c r="A41" s="24" t="s">
         <v>61</v>
       </c>
       <c r="B41" s="1" t="s">
@@ -3126,7 +3142,7 @@
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
-      <c r="H41" s="21" t="s">
+      <c r="H41" s="24" t="s">
         <v>0</v>
       </c>
       <c r="I41" s="1"/>
@@ -3137,7 +3153,7 @@
       <c r="N41" s="1"/>
       <c r="O41" s="1"/>
       <c r="P41" s="1"/>
-      <c r="Q41" s="21" t="s">
+      <c r="Q41" s="24" t="s">
         <v>0</v>
       </c>
       <c r="R41" s="1"/>
@@ -3148,10 +3164,10 @@
       <c r="W41" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="X41" s="21"/>
+      <c r="X41" s="24"/>
     </row>
     <row r="42" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="21"/>
+      <c r="A42" s="24"/>
       <c r="B42" s="1" t="s">
         <v>51</v>
       </c>
@@ -3160,7 +3176,7 @@
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
-      <c r="H42" s="21" t="s">
+      <c r="H42" s="24" t="s">
         <v>0</v>
       </c>
       <c r="I42" s="1"/>
@@ -3171,7 +3187,7 @@
       <c r="N42" s="1"/>
       <c r="O42" s="1"/>
       <c r="P42" s="1"/>
-      <c r="Q42" s="21" t="s">
+      <c r="Q42" s="24" t="s">
         <v>0</v>
       </c>
       <c r="R42" s="1"/>
@@ -3182,10 +3198,10 @@
       <c r="W42" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="X42" s="21"/>
+      <c r="X42" s="24"/>
     </row>
     <row r="43" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="21"/>
+      <c r="A43" s="24"/>
       <c r="B43" s="1" t="s">
         <v>52</v>
       </c>
@@ -3194,7 +3210,7 @@
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
-      <c r="H43" s="21" t="s">
+      <c r="H43" s="24" t="s">
         <v>0</v>
       </c>
       <c r="I43" s="1"/>
@@ -3205,7 +3221,7 @@
       <c r="N43" s="1"/>
       <c r="O43" s="1"/>
       <c r="P43" s="1"/>
-      <c r="Q43" s="21" t="s">
+      <c r="Q43" s="24" t="s">
         <v>0</v>
       </c>
       <c r="R43" s="1"/>
@@ -3216,10 +3232,10 @@
       <c r="W43" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="X43" s="21"/>
+      <c r="X43" s="24"/>
     </row>
     <row r="44" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="21"/>
+      <c r="A44" s="24"/>
       <c r="B44" s="1" t="s">
         <v>53</v>
       </c>
@@ -3228,7 +3244,7 @@
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
-      <c r="H44" s="21" t="s">
+      <c r="H44" s="24" t="s">
         <v>0</v>
       </c>
       <c r="I44" s="1"/>
@@ -3239,7 +3255,7 @@
       <c r="N44" s="1"/>
       <c r="O44" s="1"/>
       <c r="P44" s="1"/>
-      <c r="Q44" s="21" t="s">
+      <c r="Q44" s="24" t="s">
         <v>0</v>
       </c>
       <c r="R44" s="1"/>
@@ -3250,10 +3266,10 @@
       <c r="W44" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="X44" s="21"/>
+      <c r="X44" s="24"/>
     </row>
     <row r="45" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="21"/>
+      <c r="A45" s="24"/>
       <c r="B45" s="1" t="s">
         <v>54</v>
       </c>
@@ -3262,7 +3278,7 @@
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
-      <c r="H45" s="21" t="s">
+      <c r="H45" s="24" t="s">
         <v>0</v>
       </c>
       <c r="I45" s="1"/>
@@ -3273,7 +3289,7 @@
       <c r="N45" s="1"/>
       <c r="O45" s="1"/>
       <c r="P45" s="1"/>
-      <c r="Q45" s="21" t="s">
+      <c r="Q45" s="24" t="s">
         <v>0</v>
       </c>
       <c r="R45" s="1"/>
@@ -3284,10 +3300,10 @@
       <c r="W45" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="X45" s="21"/>
+      <c r="X45" s="24"/>
     </row>
     <row r="46" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="21"/>
+      <c r="A46" s="24"/>
       <c r="B46" s="1" t="s">
         <v>55</v>
       </c>
@@ -3296,7 +3312,7 @@
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
-      <c r="H46" s="21" t="s">
+      <c r="H46" s="24" t="s">
         <v>0</v>
       </c>
       <c r="I46" s="1"/>
@@ -3307,7 +3323,7 @@
       <c r="N46" s="1"/>
       <c r="O46" s="1"/>
       <c r="P46" s="1"/>
-      <c r="Q46" s="21" t="s">
+      <c r="Q46" s="24" t="s">
         <v>0</v>
       </c>
       <c r="R46" s="1"/>
@@ -3316,41 +3332,40 @@
       <c r="U46" s="1"/>
       <c r="V46" s="1"/>
       <c r="W46" s="1"/>
-      <c r="X46" s="21"/>
+      <c r="X46" s="24"/>
     </row>
     <row r="47" spans="1:24" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="20" t="s">
+      <c r="A47" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="B47" s="21"/>
-      <c r="C47" s="21"/>
-      <c r="D47" s="21"/>
-      <c r="E47" s="21"/>
-      <c r="F47" s="21"/>
-      <c r="G47" s="21"/>
-      <c r="H47" s="21"/>
-      <c r="I47" s="21"/>
-      <c r="J47" s="21"/>
-      <c r="K47" s="21"/>
-      <c r="L47" s="21"/>
-      <c r="M47" s="21"/>
-      <c r="N47" s="21"/>
-      <c r="O47" s="21"/>
-      <c r="P47" s="21"/>
-      <c r="Q47" s="21"/>
-      <c r="R47" s="21"/>
-      <c r="S47" s="21"/>
-      <c r="T47" s="21"/>
-      <c r="U47" s="21"/>
-      <c r="V47" s="21"/>
-      <c r="W47" s="21"/>
-      <c r="X47" s="21"/>
+      <c r="B47" s="24"/>
+      <c r="C47" s="24"/>
+      <c r="D47" s="24"/>
+      <c r="E47" s="24"/>
+      <c r="F47" s="24"/>
+      <c r="G47" s="24"/>
+      <c r="H47" s="24"/>
+      <c r="I47" s="24"/>
+      <c r="J47" s="24"/>
+      <c r="K47" s="24"/>
+      <c r="L47" s="24"/>
+      <c r="M47" s="24"/>
+      <c r="N47" s="24"/>
+      <c r="O47" s="24"/>
+      <c r="P47" s="24"/>
+      <c r="Q47" s="24"/>
+      <c r="R47" s="24"/>
+      <c r="S47" s="24"/>
+      <c r="T47" s="24"/>
+      <c r="U47" s="24"/>
+      <c r="V47" s="24"/>
+      <c r="W47" s="24"/>
+      <c r="X47" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="26">
     <mergeCell ref="E27:E28"/>
     <mergeCell ref="G27:G28"/>
-    <mergeCell ref="M9:M10"/>
     <mergeCell ref="A1:X1"/>
     <mergeCell ref="A2:L2"/>
     <mergeCell ref="M2:X2"/>
@@ -3358,6 +3373,7 @@
     <mergeCell ref="A11:A16"/>
     <mergeCell ref="G11:G12"/>
     <mergeCell ref="H11:H12"/>
+    <mergeCell ref="M15:M16"/>
     <mergeCell ref="A47:X47"/>
     <mergeCell ref="X5:X46"/>
     <mergeCell ref="H29:H46"/>

</xml_diff>